<commit_message>
added area budget for flash memory controller
</commit_message>
<xml_diff>
--- a/docs/AREA_BUDGET.xlsx
+++ b/docs/AREA_BUDGET.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="141">
   <si>
     <t xml:space="preserve">NAME OF BLOCK</t>
   </si>
@@ -434,9 +434,6 @@
     <t xml:space="preserve">4 Bit Flex Counter</t>
   </si>
   <si>
-    <t xml:space="preserve">Miixed</t>
-  </si>
-  <si>
     <t xml:space="preserve">8 Bit Flex Counter</t>
   </si>
   <si>
@@ -468,6 +465,39 @@
   </si>
   <si>
     <t xml:space="preserve">Shifting Logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMC Next State Logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Bit Counter Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-Bit Adder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMC State Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assume 9 states</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMC Output Logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-bit Flex Counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:1 Address Mux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:1 Data Mux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Register</t>
   </si>
 </sst>
 </file>
@@ -551,7 +581,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="34">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -783,6 +813,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -811,7 +848,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1025,6 +1062,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="33" xfId="15" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1045,10 +1098,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:O118"/>
+  <dimension ref="B1:O140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D117" activeCellId="0" sqref="D117"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C91" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N122" activeCellId="0" sqref="N122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1063,7 +1116,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="33.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.22"/>
@@ -3443,7 +3496,7 @@
         <v>118</v>
       </c>
       <c r="C98" s="51" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="D98" s="51" t="n">
         <v>25</v>
@@ -3464,7 +3517,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C99" s="51" t="s">
         <v>55</v>
@@ -3488,7 +3541,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C100" s="51" t="s">
         <v>19</v>
@@ -3512,7 +3565,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C101" s="51" t="s">
         <v>111</v>
@@ -3536,7 +3589,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C102" s="51" t="s">
         <v>111</v>
@@ -3563,7 +3616,7 @@
         <v>116</v>
       </c>
       <c r="C103" s="51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D103" s="51" t="n">
         <v>8</v>
@@ -3584,7 +3637,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C104" s="51" t="s">
         <v>19</v>
@@ -3656,7 +3709,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C107" s="51" t="s">
         <v>111</v>
@@ -3669,7 +3722,7 @@
         <v>7200</v>
       </c>
       <c r="F107" s="52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H107" s="14"/>
       <c r="I107" s="15"/>
@@ -3682,7 +3735,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C108" s="51" t="s">
         <v>111</v>
@@ -3706,7 +3759,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C109" s="51" t="s">
         <v>19</v>
@@ -3730,7 +3783,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C110" s="51" t="s">
         <v>19</v>
@@ -3778,7 +3831,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C112" s="51" t="s">
         <v>19</v>
@@ -3894,8 +3947,444 @@
       </c>
       <c r="I118" s="35"/>
     </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I120" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J120" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K120" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L120" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M120" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N120" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O120" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="1"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="H121" s="3"/>
+      <c r="I121" s="3"/>
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+      <c r="L121" s="3"/>
+      <c r="M121" s="3"/>
+      <c r="N121" s="3"/>
+      <c r="O121" s="3"/>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="C122" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D122" s="47" t="n">
+        <v>20</v>
+      </c>
+      <c r="E122" s="54" t="n">
+        <f aca="false">IF(C122="Combinational",D122*500*1.5,IF(C122="Reg. w/ Reset",D122*1600*1.5,IF(C122="Reg. w/o Reset",D122*900*1.5,IF(C122="On-chip SRAM",D122*50*1.5,"N/A"))))</f>
+        <v>15000</v>
+      </c>
+      <c r="F122" s="55"/>
+      <c r="H122" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="I122" s="9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J122" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="K122" s="9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L122" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M122" s="9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="N122" s="9" t="n">
+        <f aca="false">I122+K122+M122</f>
+        <v>0.7</v>
+      </c>
+      <c r="O122" s="10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="C123" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D123" s="56" t="n">
+        <v>5</v>
+      </c>
+      <c r="E123" s="54" t="n">
+        <f aca="false">IF(C123="Combinational",D123*500*1.5,IF(C123="Reg. w/ Reset",D123*1600*1.5,IF(C123="Reg. w/o Reset",D123*900*1.5,IF(C123="On-chip SRAM",D123*50*1.5,"N/A"))))</f>
+        <v>12000</v>
+      </c>
+      <c r="F123" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H123" s="8"/>
+      <c r="I123" s="9"/>
+      <c r="J123" s="9"/>
+      <c r="K123" s="9"/>
+      <c r="L123" s="9"/>
+      <c r="M123" s="9"/>
+      <c r="N123" s="9"/>
+      <c r="O123" s="10"/>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="C124" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D124" s="56" t="n">
+        <v>20</v>
+      </c>
+      <c r="E124" s="54" t="n">
+        <f aca="false">IF(C124="Combinational",D124*500*1.5,IF(C124="Reg. w/ Reset",D124*1600*1.5,IF(C124="Reg. w/o Reset",D124*900*1.5,IF(C124="On-chip SRAM",D124*50*1.5,"N/A"))))</f>
+        <v>15000</v>
+      </c>
+      <c r="F124" s="57"/>
+      <c r="H124" s="8"/>
+      <c r="I124" s="9"/>
+      <c r="J124" s="37"/>
+      <c r="K124" s="37"/>
+      <c r="L124" s="37"/>
+      <c r="M124" s="37"/>
+      <c r="N124" s="37"/>
+      <c r="O124" s="10"/>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="C125" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="D125" s="56" t="n">
+        <v>25</v>
+      </c>
+      <c r="E125" s="54" t="n">
+        <f aca="false">IF(C125="Combinational",D125*500*1.5,IF(C125="Reg. w/ Reset",D125*1600*1.5,IF(C125="Reg. w/o Reset",D125*900*1.5,IF(C125="On-chip SRAM",D125*50*1.5,"N/A"))))</f>
+        <v>60000</v>
+      </c>
+      <c r="F125" s="57"/>
+      <c r="H125" s="8"/>
+      <c r="I125" s="9"/>
+      <c r="J125" s="9"/>
+      <c r="K125" s="9"/>
+      <c r="L125" s="9"/>
+      <c r="M125" s="9"/>
+      <c r="N125" s="9"/>
+      <c r="O125" s="10"/>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="C126" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D126" s="56" t="n">
+        <v>21</v>
+      </c>
+      <c r="E126" s="54" t="n">
+        <f aca="false">IF(C126="Combinational",D126*500*1.5,IF(C126="Reg. w/ Reset",D126*1600*1.5,IF(C126="Reg. w/o Reset",D126*900*1.5,IF(C126="On-chip SRAM",D126*50*1.5,"N/A"))))</f>
+        <v>15750</v>
+      </c>
+      <c r="F126" s="57"/>
+      <c r="H126" s="8"/>
+      <c r="I126" s="9"/>
+      <c r="J126" s="9"/>
+      <c r="K126" s="9"/>
+      <c r="L126" s="9"/>
+      <c r="M126" s="9"/>
+      <c r="N126" s="9"/>
+      <c r="O126" s="10"/>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B127" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="C127" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D127" s="56" t="n">
+        <v>16</v>
+      </c>
+      <c r="E127" s="54" t="n">
+        <f aca="false">IF(C127="Combinational",D127*500*1.5,IF(C127="Reg. w/ Reset",D127*1600*1.5,IF(C127="Reg. w/o Reset",D127*900*1.5,IF(C127="On-chip SRAM",D127*50*1.5,"N/A"))))</f>
+        <v>38400</v>
+      </c>
+      <c r="F127" s="57"/>
+      <c r="H127" s="8"/>
+      <c r="I127" s="9"/>
+      <c r="J127" s="9"/>
+      <c r="K127" s="9"/>
+      <c r="L127" s="9"/>
+      <c r="M127" s="9"/>
+      <c r="N127" s="9"/>
+      <c r="O127" s="10"/>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B128" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="C128" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D128" s="56" t="n">
+        <v>21</v>
+      </c>
+      <c r="E128" s="54" t="n">
+        <f aca="false">IF(C128="Combinational",D128*500*1.5,IF(C128="Reg. w/ Reset",D128*1600*1.5,IF(C128="Reg. w/o Reset",D128*900*1.5,IF(C128="On-chip SRAM",D128*50*1.5,"N/A"))))</f>
+        <v>15750</v>
+      </c>
+      <c r="F128" s="57"/>
+      <c r="H128" s="8"/>
+      <c r="I128" s="9"/>
+      <c r="J128" s="9"/>
+      <c r="K128" s="9"/>
+      <c r="L128" s="9"/>
+      <c r="M128" s="9"/>
+      <c r="N128" s="9"/>
+      <c r="O128" s="10"/>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B129" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="C129" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D129" s="56" t="n">
+        <v>16</v>
+      </c>
+      <c r="E129" s="54" t="n">
+        <f aca="false">IF(C129="Combinational",D129*500*1.5,IF(C129="Reg. w/ Reset",D129*1600*1.5,IF(C129="Reg. w/o Reset",D129*900*1.5,IF(C129="On-chip SRAM",D129*50*1.5,"N/A"))))</f>
+        <v>38400</v>
+      </c>
+      <c r="F129" s="57"/>
+      <c r="H129" s="8"/>
+      <c r="I129" s="9"/>
+      <c r="J129" s="9"/>
+      <c r="K129" s="9"/>
+      <c r="L129" s="9"/>
+      <c r="M129" s="9"/>
+      <c r="N129" s="9"/>
+      <c r="O129" s="10"/>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B130" s="8"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="10"/>
+      <c r="H130" s="14"/>
+      <c r="I130" s="15"/>
+      <c r="J130" s="15"/>
+      <c r="K130" s="15"/>
+      <c r="L130" s="15"/>
+      <c r="M130" s="15"/>
+      <c r="N130" s="15"/>
+      <c r="O130" s="16"/>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B131" s="8"/>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="10"/>
+      <c r="H131" s="14"/>
+      <c r="I131" s="15"/>
+      <c r="J131" s="15"/>
+      <c r="K131" s="15"/>
+      <c r="L131" s="15"/>
+      <c r="M131" s="15"/>
+      <c r="N131" s="15"/>
+      <c r="O131" s="16"/>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B132" s="8"/>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="10"/>
+      <c r="H132" s="14"/>
+      <c r="I132" s="15"/>
+      <c r="J132" s="15"/>
+      <c r="K132" s="15"/>
+      <c r="L132" s="15"/>
+      <c r="M132" s="15"/>
+      <c r="N132" s="15"/>
+      <c r="O132" s="16"/>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B133" s="8"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="10"/>
+      <c r="H133" s="14"/>
+      <c r="I133" s="15"/>
+      <c r="J133" s="15"/>
+      <c r="K133" s="15"/>
+      <c r="L133" s="15"/>
+      <c r="M133" s="15"/>
+      <c r="N133" s="15"/>
+      <c r="O133" s="16"/>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B134" s="8"/>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="10"/>
+      <c r="H134" s="14"/>
+      <c r="I134" s="15"/>
+      <c r="J134" s="15"/>
+      <c r="K134" s="15"/>
+      <c r="L134" s="15"/>
+      <c r="M134" s="15"/>
+      <c r="N134" s="15"/>
+      <c r="O134" s="16"/>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B135" s="8"/>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="10"/>
+      <c r="H135" s="14"/>
+      <c r="I135" s="15"/>
+      <c r="J135" s="15"/>
+      <c r="K135" s="15"/>
+      <c r="L135" s="15"/>
+      <c r="M135" s="15"/>
+      <c r="N135" s="15"/>
+      <c r="O135" s="16"/>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B136" s="8"/>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="10"/>
+      <c r="H136" s="14"/>
+      <c r="I136" s="15"/>
+      <c r="J136" s="15"/>
+      <c r="K136" s="15"/>
+      <c r="L136" s="15"/>
+      <c r="M136" s="15"/>
+      <c r="N136" s="15"/>
+      <c r="O136" s="16"/>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B137" s="17"/>
+      <c r="C137" s="18"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="18"/>
+      <c r="F137" s="19"/>
+      <c r="H137" s="14"/>
+      <c r="I137" s="15"/>
+      <c r="J137" s="15"/>
+      <c r="K137" s="15"/>
+      <c r="L137" s="15"/>
+      <c r="M137" s="15"/>
+      <c r="N137" s="15"/>
+      <c r="O137" s="16"/>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="23"/>
+      <c r="C138" s="24"/>
+      <c r="D138" s="24"/>
+      <c r="E138" s="24"/>
+      <c r="F138" s="25"/>
+      <c r="H138" s="26"/>
+      <c r="I138" s="27"/>
+      <c r="J138" s="27"/>
+      <c r="K138" s="27"/>
+      <c r="L138" s="27"/>
+      <c r="M138" s="27"/>
+      <c r="N138" s="27"/>
+      <c r="O138" s="28"/>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C139" s="30"/>
+      <c r="D139" s="30" t="n">
+        <f aca="false">SUM(D122:D138)</f>
+        <v>144</v>
+      </c>
+      <c r="E139" s="30" t="n">
+        <f aca="false">SUM(E122:E137)</f>
+        <v>210300</v>
+      </c>
+      <c r="F139" s="31"/>
+      <c r="H139" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I139" s="33"/>
+      <c r="J139" s="33"/>
+      <c r="K139" s="33"/>
+      <c r="L139" s="33"/>
+      <c r="M139" s="33"/>
+      <c r="N139" s="33" t="n">
+        <f aca="false">SUM(N122:N130)</f>
+        <v>0.7</v>
+      </c>
+      <c r="O139" s="34"/>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H140" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="I140" s="35"/>
+    </row>
   </sheetData>
-  <mergeCells count="70">
+  <mergeCells count="84">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
@@ -3966,6 +4455,20 @@
     <mergeCell ref="N94:N95"/>
     <mergeCell ref="O94:O95"/>
     <mergeCell ref="H118:I118"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="F120:F121"/>
+    <mergeCell ref="H120:H121"/>
+    <mergeCell ref="I120:I121"/>
+    <mergeCell ref="J120:J121"/>
+    <mergeCell ref="K120:K121"/>
+    <mergeCell ref="L120:L121"/>
+    <mergeCell ref="M120:M121"/>
+    <mergeCell ref="N120:N121"/>
+    <mergeCell ref="O120:O121"/>
+    <mergeCell ref="H140:I140"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
updated values for flash mem controller
</commit_message>
<xml_diff>
--- a/docs/AREA_BUDGET.xlsx
+++ b/docs/AREA_BUDGET.xlsx
@@ -1100,8 +1100,8 @@
   </sheetPr>
   <dimension ref="B1:O140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C91" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N122" activeCellId="0" sqref="N122"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C129" activeCellId="0" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4099,14 +4099,14 @@
         <v>136</v>
       </c>
       <c r="C125" s="56" t="s">
-        <v>111</v>
+        <v>55</v>
       </c>
       <c r="D125" s="56" t="n">
         <v>25</v>
       </c>
       <c r="E125" s="54" t="n">
-        <f aca="false">IF(C125="Combinational",D125*500*1.5,IF(C125="Reg. w/ Reset",D125*1600*1.5,IF(C125="Reg. w/o Reset",D125*900*1.5,IF(C125="On-chip SRAM",D125*50*1.5,"N/A"))))</f>
-        <v>60000</v>
+        <f aca="false">500*20*1.5 +5*1600*1.5</f>
+        <v>27000</v>
       </c>
       <c r="F125" s="57"/>
       <c r="H125" s="8"/>
@@ -4360,7 +4360,7 @@
       </c>
       <c r="E139" s="30" t="n">
         <f aca="false">SUM(E122:E137)</f>
-        <v>210300</v>
+        <v>177300</v>
       </c>
       <c r="F139" s="31"/>
       <c r="H139" s="32" t="s">

</xml_diff>